<commit_message>
morning session day 7
</commit_message>
<xml_diff>
--- a/Day 6/LP Excel/Book1.xlsx
+++ b/Day 6/LP Excel/Book1.xlsx
@@ -4,90 +4,188 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="15315" windowHeight="6735" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="15315" windowHeight="6735" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Basic" sheetId="1" r:id="rId1"/>
     <sheet name="Bottle Prblm" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Manuf Prblm" sheetId="3" r:id="rId3"/>
+    <sheet name="Shampoo Prblm" sheetId="4" r:id="rId4"/>
+    <sheet name="Farm Prblm" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Basic!$E$4:$F$4</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">'Bottle Prblm'!$E$4:$F$4</definedName>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">'Farm Prblm'!$E$4:$F$4</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">'Manuf Prblm'!$E$4:$F$4</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">'Shampoo Prblm'!$E$4:$F$4</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Basic!$G$6:$G$8</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Bottle Prblm'!$G$11:$G$12</definedName>
+    <definedName name="solver_lhs1" localSheetId="4" hidden="1">'Farm Prblm'!$G$6:$G$7</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'Manuf Prblm'!$G$6:$G$8</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">'Shampoo Prblm'!$G$6:$G$8</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">Basic!$G$8</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Bottle Prblm'!$G$6:$G$8</definedName>
+    <definedName name="solver_lhs2" localSheetId="4" hidden="1">'Farm Prblm'!$G$9</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">'Manuf Prblm'!$G$6:$G$8</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">Basic!$G$8</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Basic!$G$4</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">'Bottle Prblm'!$G$4</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">'Farm Prblm'!$G$4</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">'Manuf Prblm'!$G$4</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">'Shampoo Prblm'!$G$4</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">Basic!$I$6:$I$8</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">'Bottle Prblm'!$I$11:$I$12</definedName>
+    <definedName name="solver_rhs1" localSheetId="4" hidden="1">'Farm Prblm'!$I$6:$I$7</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">'Manuf Prblm'!$I$6:$I$8</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">'Shampoo Prblm'!$I$6:$I$8</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">Basic!$I$8</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">'Bottle Prblm'!$I$6:$I$8</definedName>
+    <definedName name="solver_rhs2" localSheetId="4" hidden="1">'Farm Prblm'!$I$9</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">'Manuf Prblm'!$I$6:$I$8</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">Basic!$I$8</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
   <si>
     <t>x1</t>
   </si>
@@ -132,13 +230,61 @@
   </si>
   <si>
     <t xml:space="preserve">Days in April </t>
+  </si>
+  <si>
+    <t>Part A</t>
+  </si>
+  <si>
+    <t>Part B</t>
+  </si>
+  <si>
+    <t>Lathes</t>
+  </si>
+  <si>
+    <t>Milling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grinding </t>
+  </si>
+  <si>
+    <t>minimzation problem</t>
+  </si>
+  <si>
+    <t>Plant I</t>
+  </si>
+  <si>
+    <t>Plant II</t>
+  </si>
+  <si>
+    <t>Fresh</t>
+  </si>
+  <si>
+    <t>Blossom</t>
+  </si>
+  <si>
+    <t>Moon</t>
+  </si>
+  <si>
+    <t>Corn</t>
+  </si>
+  <si>
+    <t>Soyabean</t>
+  </si>
+  <si>
+    <t>Protein</t>
+  </si>
+  <si>
+    <t>Fibre</t>
+  </si>
+  <si>
+    <t>Daily</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +299,32 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Book Antiqua"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Book Antiqua"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -193,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -209,6 +381,38 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -515,7 +719,7 @@
   <dimension ref="D3:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="A1:XFD1048576"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,10 +848,194 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:I12"/>
+  <dimension ref="D2:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6:H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D3" s="2"/>
+      <c r="E3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
+      <c r="E4" s="4">
+        <v>11.999999999999998</v>
+      </c>
+      <c r="F4" s="4">
+        <v>4.0000000000000009</v>
+      </c>
+      <c r="G4" s="5">
+        <f>SUMPRODUCT(E4:F4, E5:F5)</f>
+        <v>8800</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>600</v>
+      </c>
+      <c r="F5" s="2">
+        <v>400</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1500</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1500</v>
+      </c>
+      <c r="G6" s="6">
+        <f>SUMPRODUCT(E6:F6, E4:F4)</f>
+        <v>23999.999999999996</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="2">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="7" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2">
+        <v>3000</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1000</v>
+      </c>
+      <c r="G7" s="6">
+        <f>SUMPRODUCT(E7:F7, E4:F4)</f>
+        <v>39999.999999999993</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="2">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="8" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2000</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G8" s="6">
+        <f>SUMPRODUCT(E8:F8, E4:F4)</f>
+        <v>44000</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="2">
+        <v>44000</v>
+      </c>
+    </row>
+    <row r="9" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="11" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <f>SUMPRODUCT(E11:F11,E4:F4)</f>
+        <v>11.999999999999998</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <f>SUMPRODUCT(E12:F12,E4:F4)</f>
+        <v>4.0000000000000009</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="2">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D2:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,10 +1048,10 @@
   <sheetData>
     <row r="2" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -684,14 +1072,14 @@
     <row r="4" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="4">
-        <v>11.999999999999998</v>
+        <v>0</v>
       </c>
       <c r="F4" s="4">
-        <v>4.0000000000000009</v>
+        <v>200</v>
       </c>
       <c r="G4" s="5">
         <f>SUMPRODUCT(E4:F4, E5:F5)</f>
-        <v>8800</v>
+        <v>20000</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -699,10 +1087,10 @@
     <row r="5" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
       <c r="E5" s="2">
-        <v>600</v>
+        <v>40</v>
       </c>
       <c r="F5" s="2">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -710,65 +1098,65 @@
     </row>
     <row r="6" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E6" s="2">
-        <v>1500</v>
+        <v>12</v>
       </c>
       <c r="F6" s="2">
-        <v>1500</v>
+        <v>6</v>
       </c>
       <c r="G6" s="6">
         <f>SUMPRODUCT(E6:F6, E4:F4)</f>
-        <v>23999.999999999996</v>
+        <v>1200</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="I6" s="2">
-        <v>20000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="7" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E7" s="2">
-        <v>3000</v>
+        <v>4</v>
       </c>
       <c r="F7" s="2">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="G7" s="6">
         <f>SUMPRODUCT(E7:F7, E4:F4)</f>
-        <v>39999.999999999993</v>
+        <v>2000</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="I7" s="2">
-        <v>40000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="8" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D8" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E8" s="2">
-        <v>2000</v>
+        <v>2</v>
       </c>
       <c r="F8" s="2">
-        <v>5000</v>
+        <v>3</v>
       </c>
       <c r="G8" s="6">
         <f>SUMPRODUCT(E8:F8, E4:F4)</f>
-        <v>44000</v>
+        <v>600</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="I8" s="2">
-        <v>44000</v>
+        <v>900</v>
       </c>
     </row>
     <row r="9" spans="4:9" x14ac:dyDescent="0.25">
@@ -779,60 +1167,298 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <f>SUMPRODUCT(E11:F11,E4:F4)</f>
-        <v>11.999999999999998</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I11" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1">
-        <f>SUMPRODUCT(E12:F12,E4:F4)</f>
-        <v>4.0000000000000009</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12" s="2">
-        <v>30</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="D2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="F5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="9.140625" style="7"/>
+    <col min="4" max="4" width="14" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="E2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D3" s="8"/>
+      <c r="E3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D4" s="8"/>
+      <c r="E4" s="10">
+        <v>3.9999999999999982</v>
+      </c>
+      <c r="F4" s="10">
+        <v>11.999999999999996</v>
+      </c>
+      <c r="G4" s="11">
+        <f>SUMPRODUCT(E4:F4, E5:F5)</f>
+        <v>9399.9999999999964</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D5" s="8"/>
+      <c r="E5" s="8">
+        <v>700</v>
+      </c>
+      <c r="F5" s="8">
+        <v>550</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="8">
+        <v>3000</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1000</v>
+      </c>
+      <c r="G6" s="12">
+        <f>SUMPRODUCT(E6:F6, E4:F4)</f>
+        <v>23999.999999999993</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="8">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="8">
+        <v>1000</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1000</v>
+      </c>
+      <c r="G7" s="12">
+        <f>SUMPRODUCT(E7:F7, E4:F4)</f>
+        <v>15999.999999999995</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="8">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="8">
+        <v>2000</v>
+      </c>
+      <c r="F8" s="8">
+        <v>6000</v>
+      </c>
+      <c r="G8" s="12">
+        <f>SUMPRODUCT(E8:F8, E4:F4)</f>
+        <v>79999.999999999985</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="8">
+        <v>48000</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D2:I9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="9.140625" style="13"/>
+    <col min="4" max="4" width="13.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="E2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D3" s="14"/>
+      <c r="E3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D4" s="14"/>
+      <c r="E4" s="16">
+        <v>470.58823529411768</v>
+      </c>
+      <c r="F4" s="16">
+        <v>329.41176470588232</v>
+      </c>
+      <c r="G4" s="17">
+        <f>SUMPRODUCT(E4:F4, E5:F5)</f>
+        <v>437.64705882352939</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+    </row>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D5" s="14"/>
+      <c r="E5" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="F5" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D6" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0.09</v>
+      </c>
+      <c r="F6" s="14">
+        <v>0.6</v>
+      </c>
+      <c r="G6" s="18">
+        <f>SUMPRODUCT(E6:F6, E4:F4)</f>
+        <v>239.99999999999997</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="14">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D7" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="14">
+        <v>1</v>
+      </c>
+      <c r="F7" s="14">
+        <v>1</v>
+      </c>
+      <c r="G7" s="18">
+        <f>SUMPRODUCT(E7:F7, E4:F4)</f>
+        <v>800</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="14">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D9" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="14">
+        <v>0.02</v>
+      </c>
+      <c r="F9" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="G9" s="18">
+        <f>SUMPRODUCT(E9:F9, E4:F4)</f>
+        <v>29.17647058823529</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="14">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>